<commit_message>
Ordering into modules write and read
</commit_message>
<xml_diff>
--- a/Assets/MANAGER_TABLES/7116301002.0.xlsx
+++ b/Assets/MANAGER_TABLES/7116301002.0.xlsx
@@ -345,7 +345,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -355,417 +355,337 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="n">
-        <v>772511104</v>
+        <v>5469981294</v>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>Regan</t>
+          <t>Jena</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>Saundra</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>B</t>
-        </is>
+          <t>Katie</t>
+        </is>
+      </c>
+      <c r="D1" t="n">
+        <v>1386825528</v>
       </c>
       <c r="E1" t="n">
-        <v>7285813456</v>
-      </c>
-      <c r="F1" t="n">
         <v>7116301002</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>1840813154</v>
+        <v>8183209510</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Michiko</t>
+          <t>Chu</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Vern</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
+          <t>Ashlee</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>1386825528</v>
       </c>
       <c r="E2" t="n">
-        <v>7285813456</v>
-      </c>
-      <c r="F2" t="n">
         <v>7116301002</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>6196104902</v>
+        <v>1659015005</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Dorinda</t>
+          <t>Argentina</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Tony</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>D</t>
-        </is>
+          <t>Josephina</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>1386825528</v>
       </c>
       <c r="E3" t="n">
-        <v>7285813456</v>
-      </c>
-      <c r="F3" t="n">
         <v>7116301002</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>8174287788</v>
+        <v>5806893864</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Isadora</t>
+          <t>Jess</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Felisa</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>D</t>
-        </is>
+          <t>Franklyn</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>1386825528</v>
       </c>
       <c r="E4" t="n">
-        <v>7285813456</v>
-      </c>
-      <c r="F4" t="n">
         <v>7116301002</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>8392664187</v>
+        <v>3789262285</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Fabiola</t>
+          <t>Lorina</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Ilona</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
+          <t>Melanie</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>1386825528</v>
       </c>
       <c r="E5" t="n">
-        <v>7285813456</v>
-      </c>
-      <c r="F5" t="n">
         <v>7116301002</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>8869537355</v>
+        <v>1907605661</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Sina</t>
+          <t>Shaunte</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Jamee</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
+          <t>Maurine</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>1386825528</v>
       </c>
       <c r="E6" t="n">
-        <v>7285813456</v>
-      </c>
-      <c r="F6" t="n">
         <v>7116301002</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>5469981294</v>
+        <v>8791567243</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Jena</t>
+          <t>Marcelene</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Katie</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
+          <t>Natasha</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>1386825528</v>
       </c>
       <c r="E7" t="n">
-        <v>1386825528</v>
-      </c>
-      <c r="F7" t="n">
         <v>7116301002</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>8183209510</v>
+        <v>6791023970</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Chu</t>
+          <t>Tashina</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Ashlee</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
+          <t>Dan</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>1386825528</v>
       </c>
       <c r="E8" t="n">
-        <v>1386825528</v>
-      </c>
-      <c r="F8" t="n">
         <v>7116301002</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>1659015005</v>
+        <v>8322067705</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Argentina</t>
+          <t>Derick</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Josephina</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>B</t>
-        </is>
+          <t>Elinor</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>1386825528</v>
       </c>
       <c r="E9" t="n">
-        <v>1386825528</v>
-      </c>
-      <c r="F9" t="n">
         <v>7116301002</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>5806893864</v>
+        <v>772511104</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Jess</t>
+          <t>Regan</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Franklyn</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
+          <t>Saundra</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>7285813456</v>
       </c>
       <c r="E10" t="n">
-        <v>1386825528</v>
-      </c>
-      <c r="F10" t="n">
         <v>7116301002</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>3789262285</v>
+        <v>1840813154</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Lorina</t>
+          <t>Michiko</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Melanie</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
+          <t>Vern</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>7285813456</v>
       </c>
       <c r="E11" t="n">
-        <v>1386825528</v>
-      </c>
-      <c r="F11" t="n">
         <v>7116301002</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>1907605661</v>
+        <v>6196104902</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Shaunte</t>
+          <t>Dorinda</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Maurine</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
+          <t>Tony</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>7285813456</v>
       </c>
       <c r="E12" t="n">
-        <v>1386825528</v>
-      </c>
-      <c r="F12" t="n">
         <v>7116301002</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>8791567243</v>
+        <v>8174287788</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Marcelene</t>
+          <t>Isadora</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Natasha</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>B</t>
-        </is>
+          <t>Felisa</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>7285813456</v>
       </c>
       <c r="E13" t="n">
-        <v>1386825528</v>
-      </c>
-      <c r="F13" t="n">
         <v>7116301002</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>6791023970</v>
+        <v>8392664187</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Tashina</t>
+          <t>Fabiola</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Dan</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
+          <t>Ilona</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>7285813456</v>
       </c>
       <c r="E14" t="n">
-        <v>1386825528</v>
-      </c>
-      <c r="F14" t="n">
         <v>7116301002</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>8322067705</v>
+        <v>8869537355</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Derick</t>
+          <t>Sina</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Elinor</t>
-        </is>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
+          <t>Jamee</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>7285813456</v>
       </c>
       <c r="E15" t="n">
-        <v>1386825528</v>
-      </c>
-      <c r="F15" t="n">
         <v>7116301002</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>47708660</v>
+        <v>32039648</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Anette</t>
+          <t>Luciana</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Myra</t>
-        </is>
-      </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>B</t>
-        </is>
+          <t>Isabella</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>7285813456</v>
       </c>
       <c r="E16" t="n">
-        <v>1386825528</v>
-      </c>
-      <c r="F16" t="n">
         <v>7116301002</v>
       </c>
     </row>

</xml_diff>

<commit_message>
changing names and moving append to writer
</commit_message>
<xml_diff>
--- a/Assets/MANAGER_TABLES/7116301002.0.xlsx
+++ b/Assets/MANAGER_TABLES/7116301002.0.xlsx
@@ -345,7 +345,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:E46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -670,22 +670,652 @@
     </row>
     <row r="16">
       <c r="A16" t="n">
+        <v>5469981294</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Jena</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Katie</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>1386825528</v>
+      </c>
+      <c r="E16" t="n">
+        <v>7116301002</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>8183209510</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Chu</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Ashlee</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>1386825528</v>
+      </c>
+      <c r="E17" t="n">
+        <v>7116301002</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>1659015005</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Argentina</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Josephina</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>1386825528</v>
+      </c>
+      <c r="E18" t="n">
+        <v>7116301002</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>5806893864</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Jess</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Franklyn</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
+        <v>1386825528</v>
+      </c>
+      <c r="E19" t="n">
+        <v>7116301002</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>3789262285</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Lorina</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Melanie</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>1386825528</v>
+      </c>
+      <c r="E20" t="n">
+        <v>7116301002</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>1907605661</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Shaunte</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Maurine</t>
+        </is>
+      </c>
+      <c r="D21" t="n">
+        <v>1386825528</v>
+      </c>
+      <c r="E21" t="n">
+        <v>7116301002</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>8791567243</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Marcelene</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Natasha</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
+        <v>1386825528</v>
+      </c>
+      <c r="E22" t="n">
+        <v>7116301002</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>6791023970</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Tashina</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>Dan</t>
+        </is>
+      </c>
+      <c r="D23" t="n">
+        <v>1386825528</v>
+      </c>
+      <c r="E23" t="n">
+        <v>7116301002</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>8322067705</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Derick</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>Elinor</t>
+        </is>
+      </c>
+      <c r="D24" t="n">
+        <v>1386825528</v>
+      </c>
+      <c r="E24" t="n">
+        <v>7116301002</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>772511104</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Regan</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>Saundra</t>
+        </is>
+      </c>
+      <c r="D25" t="n">
+        <v>7285813456</v>
+      </c>
+      <c r="E25" t="n">
+        <v>7116301002</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>1840813154</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Michiko</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>Vern</t>
+        </is>
+      </c>
+      <c r="D26" t="n">
+        <v>7285813456</v>
+      </c>
+      <c r="E26" t="n">
+        <v>7116301002</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>6196104902</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Dorinda</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>Tony</t>
+        </is>
+      </c>
+      <c r="D27" t="n">
+        <v>7285813456</v>
+      </c>
+      <c r="E27" t="n">
+        <v>7116301002</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>8174287788</v>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Isadora</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>Felisa</t>
+        </is>
+      </c>
+      <c r="D28" t="n">
+        <v>7285813456</v>
+      </c>
+      <c r="E28" t="n">
+        <v>7116301002</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>8392664187</v>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>Fabiola</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>Ilona</t>
+        </is>
+      </c>
+      <c r="D29" t="n">
+        <v>7285813456</v>
+      </c>
+      <c r="E29" t="n">
+        <v>7116301002</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>8869537355</v>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Sina</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>Jamee</t>
+        </is>
+      </c>
+      <c r="D30" t="n">
+        <v>7285813456</v>
+      </c>
+      <c r="E30" t="n">
+        <v>7116301002</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>5469981294</v>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>Jena</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>Katie</t>
+        </is>
+      </c>
+      <c r="D31" t="n">
+        <v>1386825528</v>
+      </c>
+      <c r="E31" t="n">
+        <v>7116301002</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>8183209510</v>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>Chu</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>Ashlee</t>
+        </is>
+      </c>
+      <c r="D32" t="n">
+        <v>1386825528</v>
+      </c>
+      <c r="E32" t="n">
+        <v>7116301002</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>1659015005</v>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>Argentina</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>Josephina</t>
+        </is>
+      </c>
+      <c r="D33" t="n">
+        <v>1386825528</v>
+      </c>
+      <c r="E33" t="n">
+        <v>7116301002</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>5806893864</v>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>Jess</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>Franklyn</t>
+        </is>
+      </c>
+      <c r="D34" t="n">
+        <v>1386825528</v>
+      </c>
+      <c r="E34" t="n">
+        <v>7116301002</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>3789262285</v>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>Lorina</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>Melanie</t>
+        </is>
+      </c>
+      <c r="D35" t="n">
+        <v>1386825528</v>
+      </c>
+      <c r="E35" t="n">
+        <v>7116301002</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>1907605661</v>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>Shaunte</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>Maurine</t>
+        </is>
+      </c>
+      <c r="D36" t="n">
+        <v>1386825528</v>
+      </c>
+      <c r="E36" t="n">
+        <v>7116301002</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>8791567243</v>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>Marcelene</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>Natasha</t>
+        </is>
+      </c>
+      <c r="D37" t="n">
+        <v>1386825528</v>
+      </c>
+      <c r="E37" t="n">
+        <v>7116301002</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>6791023970</v>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>Tashina</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>Dan</t>
+        </is>
+      </c>
+      <c r="D38" t="n">
+        <v>1386825528</v>
+      </c>
+      <c r="E38" t="n">
+        <v>7116301002</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>8322067705</v>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>Derick</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>Elinor</t>
+        </is>
+      </c>
+      <c r="D39" t="n">
+        <v>1386825528</v>
+      </c>
+      <c r="E39" t="n">
+        <v>7116301002</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>772511104</v>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>Regan</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>Saundra</t>
+        </is>
+      </c>
+      <c r="D40" t="n">
+        <v>7285813456</v>
+      </c>
+      <c r="E40" t="n">
+        <v>7116301002</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>1840813154</v>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>Michiko</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>Vern</t>
+        </is>
+      </c>
+      <c r="D41" t="n">
+        <v>7285813456</v>
+      </c>
+      <c r="E41" t="n">
+        <v>7116301002</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>6196104902</v>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>Dorinda</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>Tony</t>
+        </is>
+      </c>
+      <c r="D42" t="n">
+        <v>7285813456</v>
+      </c>
+      <c r="E42" t="n">
+        <v>7116301002</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>8174287788</v>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>Isadora</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>Felisa</t>
+        </is>
+      </c>
+      <c r="D43" t="n">
+        <v>7285813456</v>
+      </c>
+      <c r="E43" t="n">
+        <v>7116301002</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n">
+        <v>8392664187</v>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>Fabiola</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>Ilona</t>
+        </is>
+      </c>
+      <c r="D44" t="n">
+        <v>7285813456</v>
+      </c>
+      <c r="E44" t="n">
+        <v>7116301002</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="n">
+        <v>8869537355</v>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>Sina</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>Jamee</t>
+        </is>
+      </c>
+      <c r="D45" t="n">
+        <v>7285813456</v>
+      </c>
+      <c r="E45" t="n">
+        <v>7116301002</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="n">
         <v>32039648</v>
       </c>
-      <c r="B16" t="inlineStr">
+      <c r="B46" t="inlineStr">
         <is>
           <t>Luciana</t>
         </is>
       </c>
-      <c r="C16" t="inlineStr">
+      <c r="C46" t="inlineStr">
         <is>
           <t>Isabella</t>
         </is>
       </c>
-      <c r="D16" t="n">
-        <v>7285813456</v>
-      </c>
-      <c r="E16" t="n">
+      <c r="D46" t="n">
+        <v>7285813456</v>
+      </c>
+      <c r="E46" t="n">
         <v>7116301002</v>
       </c>
     </row>

</xml_diff>